<commit_message>
vizualizare repartizare din administrator
</commit_message>
<xml_diff>
--- a/website/Repartizare.xlsx
+++ b/website/Repartizare.xlsx
@@ -62,42 +62,42 @@
     <t>uid016</t>
   </si>
   <si>
+    <t>uid023</t>
+  </si>
+  <si>
+    <t>uid017</t>
+  </si>
+  <si>
+    <t>uid026</t>
+  </si>
+  <si>
+    <t>uid019</t>
+  </si>
+  <si>
     <t>uid025</t>
   </si>
   <si>
-    <t>uid017</t>
+    <t>uid020</t>
+  </si>
+  <si>
+    <t>uid022</t>
   </si>
   <si>
     <t>uid021</t>
   </si>
   <si>
-    <t>uid019</t>
-  </si>
-  <si>
-    <t>uid026</t>
-  </si>
-  <si>
-    <t>uid020</t>
-  </si>
-  <si>
-    <t>uid023</t>
-  </si>
-  <si>
-    <t>uid022</t>
+    <t>uid027</t>
+  </si>
+  <si>
+    <t>uid029</t>
   </si>
   <si>
     <t>uid024</t>
   </si>
   <si>
-    <t>uid027</t>
-  </si>
-  <si>
     <t>uid028</t>
   </si>
   <si>
-    <t>uid029</t>
-  </si>
-  <si>
     <t>uid030</t>
   </si>
   <si>
@@ -110,40 +110,40 @@
     <t>uid002</t>
   </si>
   <si>
+    <t>uid003</t>
+  </si>
+  <si>
+    <t>uid006</t>
+  </si>
+  <si>
+    <t>uid004</t>
+  </si>
+  <si>
+    <t>uid005</t>
+  </si>
+  <si>
+    <t>uid008</t>
+  </si>
+  <si>
+    <t>uid011</t>
+  </si>
+  <si>
+    <t>uid007</t>
+  </si>
+  <si>
     <t>uid009</t>
   </si>
   <si>
+    <t>uid012</t>
+  </si>
+  <si>
+    <t>uid013</t>
+  </si>
+  <si>
+    <t>uid014</t>
+  </si>
+  <si>
     <t>uid010</t>
-  </si>
-  <si>
-    <t>uid008</t>
-  </si>
-  <si>
-    <t>uid003</t>
-  </si>
-  <si>
-    <t>uid004</t>
-  </si>
-  <si>
-    <t>uid005</t>
-  </si>
-  <si>
-    <t>uid006</t>
-  </si>
-  <si>
-    <t>uid007</t>
-  </si>
-  <si>
-    <t>uid011</t>
-  </si>
-  <si>
-    <t>uid012</t>
-  </si>
-  <si>
-    <t>uid013</t>
-  </si>
-  <si>
-    <t>uid014</t>
   </si>
 </sst>
 </file>
@@ -851,9 +851,6 @@
       <c r="F17" t="s">
         <v>28</v>
       </c>
-      <c r="G17" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18">
@@ -863,19 +860,19 @@
         <v>5</v>
       </c>
       <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
         <v>30</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>31</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>32</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>33</v>
-      </c>
-      <c r="G18" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -886,15 +883,18 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
         <v>35</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>36</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>37</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
set mare de date testat(ok)
</commit_message>
<xml_diff>
--- a/website/Repartizare.xlsx
+++ b/website/Repartizare.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="191">
   <si>
     <t>C1</t>
   </si>
@@ -53,97 +53,553 @@
     <t>Student5</t>
   </si>
   <si>
+    <t>uid016</t>
+  </si>
+  <si>
+    <t>uid020</t>
+  </si>
+  <si>
+    <t>uid019</t>
+  </si>
+  <si>
+    <t>uid023</t>
+  </si>
+  <si>
+    <t>34135791SL197753</t>
+  </si>
+  <si>
+    <t>uid022</t>
+  </si>
+  <si>
+    <t>18965761SL326648</t>
+  </si>
+  <si>
+    <t>uid028</t>
+  </si>
+  <si>
+    <t>35642432SL652871</t>
+  </si>
+  <si>
+    <t>uid029</t>
+  </si>
+  <si>
+    <t>50631995SL276645</t>
+  </si>
+  <si>
+    <t>63509146SL539202</t>
+  </si>
+  <si>
+    <t>25273443SL017796</t>
+  </si>
+  <si>
+    <t>30190568SL563297</t>
+  </si>
+  <si>
+    <t>82294501SL694973</t>
+  </si>
+  <si>
     <t>uid015</t>
   </si>
   <si>
+    <t>uid017</t>
+  </si>
+  <si>
+    <t>57495410SL741636</t>
+  </si>
+  <si>
     <t>uid018</t>
   </si>
   <si>
-    <t>uid016</t>
-  </si>
-  <si>
-    <t>uid023</t>
-  </si>
-  <si>
-    <t>uid017</t>
+    <t>30195351SL347669</t>
+  </si>
+  <si>
+    <t>52166059SL323154</t>
+  </si>
+  <si>
+    <t>uid021</t>
+  </si>
+  <si>
+    <t>41599445SL681739</t>
+  </si>
+  <si>
+    <t>51499966SL699883</t>
+  </si>
+  <si>
+    <t>uid025</t>
+  </si>
+  <si>
+    <t>28380917SL389219</t>
+  </si>
+  <si>
+    <t>44257137SL279941</t>
   </si>
   <si>
     <t>uid026</t>
   </si>
   <si>
-    <t>uid019</t>
-  </si>
-  <si>
-    <t>uid025</t>
-  </si>
-  <si>
-    <t>uid020</t>
-  </si>
-  <si>
-    <t>uid022</t>
-  </si>
-  <si>
-    <t>uid021</t>
+    <t>15842683SL390433</t>
+  </si>
+  <si>
+    <t>66013242SL954907</t>
+  </si>
+  <si>
+    <t>uid030</t>
+  </si>
+  <si>
+    <t>42057692SL299670</t>
+  </si>
+  <si>
+    <t>68975822SL706864</t>
+  </si>
+  <si>
+    <t>89349620SL379829</t>
+  </si>
+  <si>
+    <t>32121297SL449334</t>
+  </si>
+  <si>
+    <t>46942216SL886820</t>
   </si>
   <si>
     <t>uid027</t>
   </si>
   <si>
-    <t>uid029</t>
-  </si>
-  <si>
-    <t>uid024</t>
-  </si>
-  <si>
-    <t>uid028</t>
-  </si>
-  <si>
-    <t>uid030</t>
+    <t>17847814SL202207</t>
+  </si>
+  <si>
+    <t>88735822SL773551</t>
+  </si>
+  <si>
+    <t>92330658SL960568</t>
+  </si>
+  <si>
+    <t>34491587SL582059</t>
+  </si>
+  <si>
+    <t>61682820SL870164</t>
+  </si>
+  <si>
+    <t>64954713SL567938</t>
+  </si>
+  <si>
+    <t>80700290SL680610</t>
+  </si>
+  <si>
+    <t>83260344SL252788</t>
+  </si>
+  <si>
+    <t>94480187SL488823</t>
+  </si>
+  <si>
+    <t>44847016SL812755</t>
+  </si>
+  <si>
+    <t>62529481SL112181</t>
+  </si>
+  <si>
+    <t>77338516SL279370</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>55999872SL763534</t>
+  </si>
+  <si>
+    <t>99319418SL346551</t>
+  </si>
+  <si>
+    <t>35878214SL960874</t>
+  </si>
+  <si>
+    <t>67136228SL874191</t>
+  </si>
+  <si>
+    <t>50251190SL568866</t>
+  </si>
+  <si>
+    <t>76440173SL196054</t>
+  </si>
+  <si>
+    <t>25846278SL244025</t>
+  </si>
+  <si>
+    <t>56791403SL835379</t>
+  </si>
+  <si>
+    <t>22926803SL462735</t>
+  </si>
+  <si>
+    <t>88008006SL259077</t>
+  </si>
+  <si>
+    <t>71239430SL300166</t>
+  </si>
+  <si>
+    <t>98309373SL855419</t>
+  </si>
+  <si>
+    <t>49090482SL142574</t>
+  </si>
+  <si>
+    <t>64719938SL261631</t>
+  </si>
+  <si>
+    <t>52806352SL995133</t>
+  </si>
+  <si>
+    <t>54439397SL898689</t>
+  </si>
+  <si>
+    <t>44237247SL125812</t>
+  </si>
+  <si>
+    <t>62322059SL269300</t>
+  </si>
+  <si>
+    <t>12406190SL536683</t>
+  </si>
+  <si>
+    <t>90866177SL052120</t>
+  </si>
+  <si>
+    <t>19466485SL864106</t>
+  </si>
+  <si>
+    <t>31747473SL526466</t>
+  </si>
+  <si>
+    <t>32622952SL655972</t>
+  </si>
+  <si>
+    <t>34380082SL485901</t>
+  </si>
+  <si>
+    <t>89418815SL526598</t>
+  </si>
+  <si>
+    <t>70519776SL816097</t>
+  </si>
+  <si>
+    <t>79982869SL564627</t>
+  </si>
+  <si>
+    <t>86853038SL091859</t>
+  </si>
+  <si>
+    <t>12063590SL153795</t>
+  </si>
+  <si>
+    <t>66833378SL837113</t>
+  </si>
+  <si>
+    <t>76736132SL334663</t>
+  </si>
+  <si>
+    <t>17943651SL990247</t>
+  </si>
+  <si>
+    <t>28298182SL537367</t>
+  </si>
+  <si>
+    <t>52684318SL429707</t>
+  </si>
+  <si>
+    <t>13843074SL831290</t>
+  </si>
+  <si>
+    <t>21428852SL194893</t>
+  </si>
+  <si>
+    <t>85715700SL752833</t>
+  </si>
+  <si>
+    <t>20437170SL046570</t>
+  </si>
+  <si>
+    <t>36547397SL570586</t>
+  </si>
+  <si>
+    <t>48811034SL542666</t>
   </si>
   <si>
     <t>C12</t>
   </si>
   <si>
+    <t>74448284SL002199</t>
+  </si>
+  <si>
+    <t>87841762SL090008</t>
+  </si>
+  <si>
+    <t>uid012</t>
+  </si>
+  <si>
+    <t>uid013</t>
+  </si>
+  <si>
+    <t>62633881SL211127</t>
+  </si>
+  <si>
+    <t>14133564SL637573</t>
+  </si>
+  <si>
+    <t>30600157SL948669</t>
+  </si>
+  <si>
+    <t>43465435SL914016</t>
+  </si>
+  <si>
+    <t>66545279SL527587</t>
+  </si>
+  <si>
+    <t>16560888SL989953</t>
+  </si>
+  <si>
+    <t>77911337SL719827</t>
+  </si>
+  <si>
+    <t>86602839SL456364</t>
+  </si>
+  <si>
+    <t>87401175SL033059</t>
+  </si>
+  <si>
+    <t>12092538SL593625</t>
+  </si>
+  <si>
+    <t>87949886SL873473</t>
+  </si>
+  <si>
+    <t>89145280SL550351</t>
+  </si>
+  <si>
+    <t>95803012SL897630</t>
+  </si>
+  <si>
     <t>uid001</t>
   </si>
   <si>
     <t>uid002</t>
   </si>
   <si>
+    <t>uid009</t>
+  </si>
+  <si>
+    <t>uid014</t>
+  </si>
+  <si>
+    <t>21319801SL222278</t>
+  </si>
+  <si>
+    <t>54904811SL267921</t>
+  </si>
+  <si>
+    <t>68079602SL971308</t>
+  </si>
+  <si>
+    <t>82148329SL730968</t>
+  </si>
+  <si>
+    <t>93899950SL775867</t>
+  </si>
+  <si>
+    <t>uid007</t>
+  </si>
+  <si>
+    <t>15777438SL604976</t>
+  </si>
+  <si>
+    <t>68496354SL167262</t>
+  </si>
+  <si>
+    <t>74027632SL920496</t>
+  </si>
+  <si>
+    <t>81904976SL969543</t>
+  </si>
+  <si>
     <t>uid003</t>
   </si>
   <si>
+    <t>uid004</t>
+  </si>
+  <si>
+    <t>uid005</t>
+  </si>
+  <si>
     <t>uid006</t>
   </si>
   <si>
-    <t>uid004</t>
-  </si>
-  <si>
-    <t>uid005</t>
+    <t>29219413SL844597</t>
+  </si>
+  <si>
+    <t>76128298SL627099</t>
   </si>
   <si>
     <t>uid008</t>
   </si>
   <si>
+    <t>uid010</t>
+  </si>
+  <si>
+    <t>20133001SL833337</t>
+  </si>
+  <si>
+    <t>55400730SL620228</t>
+  </si>
+  <si>
+    <t>64577306SL089366</t>
+  </si>
+  <si>
+    <t>80047651SL353655</t>
+  </si>
+  <si>
+    <t>25949671SL185668</t>
+  </si>
+  <si>
+    <t>69228733SL286098</t>
+  </si>
+  <si>
+    <t>91519304SL349213</t>
+  </si>
+  <si>
+    <t>95365217SL456123</t>
+  </si>
+  <si>
+    <t>87452455SL166390</t>
+  </si>
+  <si>
+    <t>57014148SL892451</t>
+  </si>
+  <si>
+    <t>79074691SL057251</t>
+  </si>
+  <si>
+    <t>92681100SL794640</t>
+  </si>
+  <si>
     <t>uid011</t>
   </si>
   <si>
-    <t>uid007</t>
-  </si>
-  <si>
-    <t>uid009</t>
-  </si>
-  <si>
-    <t>uid012</t>
-  </si>
-  <si>
-    <t>uid013</t>
-  </si>
-  <si>
-    <t>uid014</t>
-  </si>
-  <si>
-    <t>uid010</t>
+    <t>42931822SL982712</t>
+  </si>
+  <si>
+    <t>49006397SL565793</t>
+  </si>
+  <si>
+    <t>53396897SL956171</t>
+  </si>
+  <si>
+    <t>64114516SL644516</t>
+  </si>
+  <si>
+    <t>68068853SL212788</t>
+  </si>
+  <si>
+    <t>20950122SL409713</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>13264263SL015825</t>
+  </si>
+  <si>
+    <t>16420197SL572575</t>
+  </si>
+  <si>
+    <t>36034706SL390537</t>
+  </si>
+  <si>
+    <t>39314456SL851477</t>
+  </si>
+  <si>
+    <t>23456601SL556112</t>
+  </si>
+  <si>
+    <t>23598587SL471299</t>
+  </si>
+  <si>
+    <t>32093270SL100586</t>
+  </si>
+  <si>
+    <t>37529074SL095607</t>
+  </si>
+  <si>
+    <t>14911569SL294059</t>
+  </si>
+  <si>
+    <t>27519223SL112231</t>
+  </si>
+  <si>
+    <t>40607980SL517667</t>
+  </si>
+  <si>
+    <t>71046738SL708453</t>
+  </si>
+  <si>
+    <t>80209042SL879807</t>
+  </si>
+  <si>
+    <t>97149003SL464156</t>
+  </si>
+  <si>
+    <t>27404489SL974444</t>
+  </si>
+  <si>
+    <t>34213682SL748782</t>
+  </si>
+  <si>
+    <t>35895877SL565990</t>
+  </si>
+  <si>
+    <t>74004728SL830877</t>
+  </si>
+  <si>
+    <t>37278479SL825822</t>
+  </si>
+  <si>
+    <t>37374874SL140668</t>
+  </si>
+  <si>
+    <t>71514966SL687906</t>
+  </si>
+  <si>
+    <t>99015351SL057313</t>
+  </si>
+  <si>
+    <t>83481767SL254005</t>
+  </si>
+  <si>
+    <t>43720241SL357212</t>
+  </si>
+  <si>
+    <t>44094601SL299216</t>
+  </si>
+  <si>
+    <t>90943809SL570757</t>
+  </si>
+  <si>
+    <t>91165954SL777227</t>
+  </si>
+  <si>
+    <t>77634899SL249112</t>
+  </si>
+  <si>
+    <t>34187055SL882548</t>
+  </si>
+  <si>
+    <t>37371538SL799158</t>
+  </si>
+  <si>
+    <t>77873106SL079695</t>
+  </si>
+  <si>
+    <t>92310641SL118096</t>
+  </si>
+  <si>
+    <t>82087786SL300011</t>
   </si>
 </sst>
 </file>
@@ -630,7 +1086,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -742,10 +1198,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -753,211 +1209,1171 @@
       <c r="D8" t="s">
         <v>19</v>
       </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
         <v>21</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="A15">
+        <v>32</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>2</v>
+      <c r="A16">
+        <v>33</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="E16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B21">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="B22">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="B25">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26">
+        <v>43</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>44</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>45</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>20</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>21</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>22</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>23</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>24</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>25</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>26</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>70</v>
+      </c>
+      <c r="D39" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>27</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>28</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>29</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>30</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" t="s">
+        <v>79</v>
+      </c>
+      <c r="E43" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>31</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>32</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" t="s">
+        <v>84</v>
+      </c>
+      <c r="E45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>33</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" t="s">
+        <v>87</v>
+      </c>
+      <c r="E46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>34</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>89</v>
+      </c>
+      <c r="D47" t="s">
+        <v>90</v>
+      </c>
+      <c r="E47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>35</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49">
+        <v>36</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>95</v>
+      </c>
+      <c r="D49" t="s">
+        <v>96</v>
+      </c>
+      <c r="E49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50">
+        <v>37</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51">
+        <v>38</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52">
+        <v>39</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" t="s">
+        <v>5</v>
+      </c>
+      <c r="F56" t="s">
+        <v>6</v>
+      </c>
+      <c r="G56" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s">
+        <v>99</v>
+      </c>
+      <c r="D57" t="s">
+        <v>100</v>
+      </c>
+      <c r="E57" t="s">
+        <v>101</v>
+      </c>
+      <c r="F57" t="s">
+        <v>102</v>
+      </c>
+      <c r="G57" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58">
+        <v>2</v>
+      </c>
+      <c r="B58">
+        <v>5</v>
+      </c>
+      <c r="C58" t="s">
+        <v>104</v>
+      </c>
+      <c r="D58" t="s">
+        <v>105</v>
+      </c>
+      <c r="E58" t="s">
+        <v>106</v>
+      </c>
+      <c r="F58" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59">
+        <v>3</v>
+      </c>
+      <c r="B59">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s">
+        <v>108</v>
+      </c>
+      <c r="D59" t="s">
+        <v>109</v>
+      </c>
+      <c r="E59" t="s">
+        <v>110</v>
+      </c>
+      <c r="F59" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60">
+        <v>4</v>
+      </c>
+      <c r="B60">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
+        <v>112</v>
+      </c>
+      <c r="D60" t="s">
+        <v>113</v>
+      </c>
+      <c r="E60" t="s">
+        <v>114</v>
+      </c>
+      <c r="F60" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61">
+        <v>5</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>116</v>
+      </c>
+      <c r="D61" t="s">
+        <v>117</v>
+      </c>
+      <c r="E61" t="s">
+        <v>118</v>
+      </c>
+      <c r="F61" t="s">
+        <v>119</v>
+      </c>
+      <c r="G61" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62">
+        <v>6</v>
+      </c>
+      <c r="B62">
+        <v>5</v>
+      </c>
+      <c r="C62" t="s">
+        <v>121</v>
+      </c>
+      <c r="D62" t="s">
+        <v>122</v>
+      </c>
+      <c r="E62" t="s">
+        <v>123</v>
+      </c>
+      <c r="F62" t="s">
+        <v>124</v>
+      </c>
+      <c r="G62" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63">
+        <v>7</v>
+      </c>
+      <c r="B63">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>126</v>
+      </c>
+      <c r="D63" t="s">
+        <v>127</v>
+      </c>
+      <c r="E63" t="s">
+        <v>128</v>
+      </c>
+      <c r="F63" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64">
+        <v>8</v>
+      </c>
+      <c r="B64">
+        <v>5</v>
+      </c>
+      <c r="C64" t="s">
+        <v>130</v>
+      </c>
+      <c r="D64" t="s">
+        <v>131</v>
+      </c>
+      <c r="E64" t="s">
+        <v>132</v>
+      </c>
+      <c r="F64" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65">
+        <v>9</v>
+      </c>
+      <c r="B65">
+        <v>5</v>
+      </c>
+      <c r="C65" t="s">
+        <v>134</v>
+      </c>
+      <c r="D65" t="s">
+        <v>135</v>
+      </c>
+      <c r="E65" t="s">
+        <v>136</v>
+      </c>
+      <c r="F65" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66">
+        <v>10</v>
+      </c>
+      <c r="B66">
+        <v>5</v>
+      </c>
+      <c r="C66" t="s">
+        <v>138</v>
+      </c>
+      <c r="D66" t="s">
+        <v>139</v>
+      </c>
+      <c r="E66" t="s">
+        <v>140</v>
+      </c>
+      <c r="F66" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67">
+        <v>11</v>
+      </c>
+      <c r="B67">
+        <v>5</v>
+      </c>
+      <c r="C67" t="s">
+        <v>142</v>
+      </c>
+      <c r="D67" t="s">
+        <v>143</v>
+      </c>
+      <c r="E67" t="s">
+        <v>144</v>
+      </c>
+      <c r="F67" t="s">
+        <v>145</v>
+      </c>
+      <c r="G67" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68">
+        <v>12</v>
+      </c>
+      <c r="B68">
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
+        <v>147</v>
+      </c>
+      <c r="D68" t="s">
+        <v>148</v>
+      </c>
+      <c r="E68" t="s">
+        <v>149</v>
+      </c>
+      <c r="F68" t="s">
+        <v>150</v>
+      </c>
+      <c r="G68" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69">
+        <v>13</v>
+      </c>
+      <c r="B69">
+        <v>5</v>
+      </c>
+      <c r="C69" t="s">
+        <v>152</v>
+      </c>
+      <c r="D69" t="s">
+        <v>153</v>
+      </c>
+      <c r="E69" t="s">
+        <v>154</v>
+      </c>
+      <c r="F69" t="s">
+        <v>155</v>
+      </c>
+      <c r="G69" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70">
+        <v>14</v>
+      </c>
+      <c r="B70">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71">
         <v>15</v>
       </c>
-      <c r="B26">
+      <c r="B71">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
+        <v>1</v>
+      </c>
+      <c r="B75" t="s">
+        <v>2</v>
+      </c>
+      <c r="C75" t="s">
+        <v>3</v>
+      </c>
+      <c r="D75" t="s">
+        <v>4</v>
+      </c>
+      <c r="E75" t="s">
+        <v>5</v>
+      </c>
+      <c r="F75" t="s">
+        <v>6</v>
+      </c>
+      <c r="G75" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76">
+        <v>1</v>
+      </c>
+      <c r="B76">
+        <v>5</v>
+      </c>
+      <c r="C76" t="s">
+        <v>158</v>
+      </c>
+      <c r="D76" t="s">
+        <v>159</v>
+      </c>
+      <c r="E76" t="s">
+        <v>160</v>
+      </c>
+      <c r="F76" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77">
+        <v>2</v>
+      </c>
+      <c r="B77">
+        <v>5</v>
+      </c>
+      <c r="C77" t="s">
+        <v>162</v>
+      </c>
+      <c r="D77" t="s">
+        <v>163</v>
+      </c>
+      <c r="E77" t="s">
+        <v>164</v>
+      </c>
+      <c r="F77" t="s">
+        <v>165</v>
+      </c>
+      <c r="G77" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78">
+        <v>3</v>
+      </c>
+      <c r="B78">
+        <v>5</v>
+      </c>
+      <c r="C78" t="s">
+        <v>167</v>
+      </c>
+      <c r="D78" t="s">
+        <v>168</v>
+      </c>
+      <c r="E78" t="s">
+        <v>169</v>
+      </c>
+      <c r="F78" t="s">
+        <v>170</v>
+      </c>
+      <c r="G78" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79">
+        <v>4</v>
+      </c>
+      <c r="B79">
+        <v>5</v>
+      </c>
+      <c r="C79" t="s">
+        <v>172</v>
+      </c>
+      <c r="D79" t="s">
+        <v>173</v>
+      </c>
+      <c r="E79" t="s">
+        <v>174</v>
+      </c>
+      <c r="F79" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80">
+        <v>5</v>
+      </c>
+      <c r="B80">
+        <v>5</v>
+      </c>
+      <c r="C80" t="s">
+        <v>176</v>
+      </c>
+      <c r="D80" t="s">
+        <v>177</v>
+      </c>
+      <c r="E80" t="s">
+        <v>178</v>
+      </c>
+      <c r="F80" t="s">
+        <v>179</v>
+      </c>
+      <c r="G80" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81">
+        <v>6</v>
+      </c>
+      <c r="B81">
+        <v>5</v>
+      </c>
+      <c r="C81" t="s">
+        <v>181</v>
+      </c>
+      <c r="D81" t="s">
+        <v>182</v>
+      </c>
+      <c r="E81" t="s">
+        <v>183</v>
+      </c>
+      <c r="F81" t="s">
+        <v>184</v>
+      </c>
+      <c r="G81" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82">
+        <v>7</v>
+      </c>
+      <c r="B82">
+        <v>5</v>
+      </c>
+      <c r="C82" t="s">
+        <v>186</v>
+      </c>
+      <c r="D82" t="s">
+        <v>187</v>
+      </c>
+      <c r="E82" t="s">
+        <v>188</v>
+      </c>
+      <c r="F82" t="s">
+        <v>189</v>
+      </c>
+      <c r="G82" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83">
+        <v>8</v>
+      </c>
+      <c r="B83">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84">
+        <v>9</v>
+      </c>
+      <c r="B84">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85">
+        <v>10</v>
+      </c>
+      <c r="B85">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86">
+        <v>11</v>
+      </c>
+      <c r="B86">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87">
+        <v>12</v>
+      </c>
+      <c r="B87">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88">
+        <v>13</v>
+      </c>
+      <c r="B88">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89">
+        <v>14</v>
+      </c>
+      <c r="B89">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A55:G55"/>
+    <mergeCell ref="A74:G74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>